<commit_message>
support for multiple AD OUs (pipe delimited), default user location if not in AD, first run no db comparisons
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/robert_baptist_uipath_com/Documents/_ADProject/ADAutomationHubSync/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/robert_baptist_uipath_com/Documents/_ADProject/ADAutomationHubUserSync/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{D1C50650-C728-4164-9700-86A3A21720EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61AA6727-374B-4A29-8BCA-97E81D62F914}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{D1C50650-C728-4164-9700-86A3A21720EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2310E51-08EE-4C70-BEDE-86FE98CD12DD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -139,19 +139,25 @@
     <t>Bearer 93e7e0c2-2900-4ed4-9740-5d3ae7ad61e0/3f8c76bb-dcce-4dda-94ef-69bf92a16288</t>
   </si>
   <si>
-    <t>Bearer a9f39c20-843e-4b53-a1be-4e06c75e74a7/4dc29706-bed3-4273-ad3a-dbff6ba5ffb0</t>
-  </si>
-  <si>
-    <t>OU=UiPathDemo,DC=rpb,DC=local</t>
-  </si>
-  <si>
     <t>LDAPFilter</t>
   </si>
   <si>
     <t>(&amp;(objectClass=user)(objectCategory=person)(!(objectClass=computer))(!userAccountControl:1.2.840.113556.1.4.803:=2))</t>
   </si>
   <si>
-    <t>ADLocation</t>
+    <t>Bearer ab5187da-8cb5-4e8c-983e-2df947f87b6a/a4693d39-7bf1-4b39-a267-211cdaa5f4f6</t>
+  </si>
+  <si>
+    <t>ADLocations</t>
+  </si>
+  <si>
+    <t>OU=UiPathMulti1,DC=rpb,DC=local|OU=UiPathMulti2,DC=rpb,DC=local</t>
+  </si>
+  <si>
+    <t>DefaultLocationIfNone</t>
+  </si>
+  <si>
+    <t>Default Location</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -608,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -632,21 +638,28 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>